<commit_message>
#54 Edited json issue
</commit_message>
<xml_diff>
--- a/sprint_ressources/sprint3/intents_samples.xlsx
+++ b/sprint_ressources/sprint3/intents_samples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Florian\Studium\04 Faecher\10 Software Engineering\01 SE1\03 Praktikum\skillproject-di-3\sprint_ressources\sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B48346-9186-4BCA-BEE4-2D89D6628007}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6A432E-C978-458D-B42C-0CCC5DA7BA39}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11970" xr2:uid="{51FEF363-7687-4334-ADE4-02A880993692}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
   <si>
     <t>welche Kategorien gibt es</t>
   </si>
@@ -184,6 +184,21 @@
   </si>
   <si>
     <t>Nach Personenzahl</t>
+  </si>
+  <si>
+    <t>Vorlesen</t>
+  </si>
+  <si>
+    <t>Zutatenliste vorlesen</t>
+  </si>
+  <si>
+    <t>welche Zutaten brauche ich</t>
+  </si>
+  <si>
+    <t>was fuer Zutaten werden benoetigt</t>
+  </si>
+  <si>
+    <t>sag mir alle Zutatent</t>
   </si>
 </sst>
 </file>
@@ -223,7 +238,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -326,15 +341,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -346,6 +371,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -660,344 +690,509 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4DE13D8-4BEE-4240-B8FC-7ED651C9781C}">
-  <dimension ref="A2:F28"/>
+  <dimension ref="A2:F47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="8"/>
+    <col min="3" max="3" width="57" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="8"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="8"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="E10" s="8"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="E13" s="8"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="8"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="2" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A16" s="6"/>
+      <c r="B16" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="3" t="s">
+      <c r="D22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="3" t="s">
+      <c r="D23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="3" t="s">
+      <c r="D24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="3" t="s">
+      <c r="D25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="2" t="s">
+      <c r="D26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A28" s="6"/>
+      <c r="B28" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="3" t="s">
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="3" t="s">
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="3" t="s">
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="3" t="s">
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="3" t="s">
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A22" s="7"/>
-      <c r="B22" s="1" t="s">
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A35" s="6"/>
+      <c r="B35" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="2" t="s">
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D42" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="E42" s="8"/>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D43" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="9"/>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="E43" s="8"/>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D44" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="3" t="s">
+      <c r="E44" s="8"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D45" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3" t="s">
+      <c r="E45" s="8"/>
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="8"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="12"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="9"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
+    <mergeCell ref="B16:E16"/>
     <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>